<commit_message>
Restoring ability to get JSON from Excel
</commit_message>
<xml_diff>
--- a/DataSets/NorthwindOrders.xlsx
+++ b/DataSets/NorthwindOrders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adaptabletools/Code/demo/adaptableblotter-demo/DataSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adaptabletools/Code/demo-dev/DataSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0302DB-0D2E-B649-83EA-CFF4AEB1933D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F040CB82-273E-174C-A68B-E29913D8315A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="31880" windowHeight="19340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="31880" windowHeight="19320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NorthwindOrders" sheetId="1" r:id="rId1"/>
@@ -2224,7 +2224,7 @@
   <dimension ref="A1:W801"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57719,7 +57719,7 @@
         <v>61.37</v>
       </c>
       <c r="J770" s="7">
-        <f t="shared" ref="J770:J833" si="14">SUM(G770*I770)</f>
+        <f t="shared" ref="J770:J801" si="14">SUM(G770*I770)</f>
         <v>613.69999999999993</v>
       </c>
       <c r="K770" s="7">

</xml_diff>

<commit_message>
adding boolean column to northwind
</commit_message>
<xml_diff>
--- a/DataSets/NorthwindOrders.xlsx
+++ b/DataSets/NorthwindOrders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adaptabletools/Code/demo-dev/DataSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8279E3-D73C-2643-BBCE-DFD7E0B7BDD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061EE8B6-40A4-6947-BDDA-185F4675B522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="460" windowWidth="31880" windowHeight="19320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1806,9 +1806,6 @@
     <t>InvoicedCost</t>
   </si>
   <si>
-    <t>ArriveOnTime</t>
-  </si>
-  <si>
     <t>PackageCost</t>
   </si>
   <si>
@@ -1820,13 +1817,16 @@
   <si>
     <t>LastUpdatedTime</t>
   </si>
+  <si>
+    <t>IsValid</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1899,8 +1899,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2242,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2293,7 +2293,7 @@
         <v>585</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>587</v>
@@ -2302,7 +2302,7 @@
         <v>586</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>574</v>
@@ -2338,10 +2338,10 @@
         <v>583</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
@@ -6412,7 +6412,7 @@
         <v>330</v>
       </c>
       <c r="T55" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U55" t="s">
         <v>331</v>
@@ -8603,7 +8603,7 @@
         <v>330</v>
       </c>
       <c r="T84" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U84" t="s">
         <v>331</v>
@@ -10190,7 +10190,7 @@
         <v>330</v>
       </c>
       <c r="T105" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U105" t="s">
         <v>331</v>
@@ -10415,7 +10415,7 @@
         <v>330</v>
       </c>
       <c r="T108" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U108" t="s">
         <v>331</v>
@@ -23356,7 +23356,7 @@
         <v>330</v>
       </c>
       <c r="T280" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U280" t="s">
         <v>331</v>
@@ -23655,7 +23655,7 @@
         <v>330</v>
       </c>
       <c r="T284" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U284" t="s">
         <v>331</v>
@@ -28922,7 +28922,7 @@
         <v>330</v>
       </c>
       <c r="T354" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U354" t="s">
         <v>331</v>
@@ -33875,7 +33875,7 @@
         <v>330</v>
       </c>
       <c r="T420" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U420" t="s">
         <v>331</v>
@@ -40376,7 +40376,7 @@
         <v>330</v>
       </c>
       <c r="T507" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U507" t="s">
         <v>331</v>
@@ -42025,7 +42025,7 @@
         <v>330</v>
       </c>
       <c r="T529" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U529" t="s">
         <v>331</v>
@@ -53719,7 +53719,7 @@
         <v>330</v>
       </c>
       <c r="T685" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U685" t="s">
         <v>331</v>
@@ -60294,7 +60294,7 @@
         <v>330</v>
       </c>
       <c r="T773" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U773" t="s">
         <v>331</v>
@@ -60371,7 +60371,7 @@
         <v>330</v>
       </c>
       <c r="T774" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="U774" t="s">
         <v>331</v>

</xml_diff>